<commit_message>
Deploying to gh-pages from  @ 00ebb61d94de95f7b76155a9410f29199a96e0e6 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_3-1-1.xlsx
+++ b/assets/excel/2021_3-1-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C2DAD03-C0C4-43E2-9499-B592212B6A62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D627667-138B-4921-A736-BA04FE778E94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{A48FC213-52A1-46C2-A33D-ED6F8C1C4CC4}"/>
   </bookViews>
@@ -308,34 +308,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -370,10 +346,34 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -766,7 +766,7 @@
   <dimension ref="B1:J45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B6" sqref="B6:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="8.25" x14ac:dyDescent="0.15"/>
@@ -805,793 +805,793 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="10" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="32"/>
+      <c r="F7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="32"/>
+      <c r="H7" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="11"/>
+      <c r="I7" s="33"/>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="10" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="11"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="18">
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="11">
         <v>2</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="11">
         <v>3</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="11">
         <v>4</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="11">
         <v>5</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="11">
         <v>6</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="11">
         <v>7</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="12">
         <v>8</v>
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="21" t="s">
+    <row r="11" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="13">
         <v>2009</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="14">
         <v>11.9</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="14">
         <v>88.1</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="14">
         <v>6.1</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="14">
         <v>75.599999999999994</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="14">
         <v>14.4</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="14">
         <v>93.2</v>
       </c>
-      <c r="J11" s="23"/>
-    </row>
-    <row r="12" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="21" t="s">
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="13">
         <v>2009</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="14">
         <v>20.2</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="14">
         <v>91.6</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="14">
         <v>10.5</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="14">
         <v>83.6</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="14">
         <v>24.8</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="14">
         <v>95.6</v>
       </c>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="21" t="s">
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="13">
         <v>2010</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="14">
         <v>15.8</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="14">
         <v>89.5</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="14">
         <v>8</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="14">
         <v>79.3</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="14">
         <v>18.8</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="14">
         <v>92.9</v>
       </c>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="14" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="21" t="s">
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="13">
         <v>2010</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="14">
         <v>23</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="14">
         <v>92.2</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="14">
         <v>12.2</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="14">
         <v>85.7</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="14">
         <v>27.7</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="14">
         <v>94.9</v>
       </c>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="21" t="s">
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="13">
         <v>2011</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="14">
         <v>18.600000000000001</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="14">
         <v>91.6</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="14">
         <v>9.2360000000000007</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="14">
         <v>82.67</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="14">
         <v>22.46</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="14">
         <v>94.668999999999997</v>
       </c>
-      <c r="J15" s="23"/>
-    </row>
-    <row r="16" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="21" t="s">
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="13">
         <v>2011</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="14">
         <v>25.2</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="14">
         <v>93</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="14">
         <v>13.965999999999999</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="14">
         <v>84.924000000000007</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="14">
         <v>30.058</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="14">
         <v>96.557000000000002</v>
       </c>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="21" t="s">
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="13">
         <v>2012</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="14">
         <v>22.1</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="14">
         <v>92.6</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="17">
         <v>12</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="17">
         <v>79</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="17">
         <v>26</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="17">
         <v>98</v>
       </c>
-      <c r="J17" s="23"/>
-    </row>
-    <row r="18" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="21" t="s">
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="13">
         <v>2012</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="14">
         <v>27.6</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="14">
         <v>93.4</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="17">
         <v>16</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="17">
         <v>87</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="17">
         <v>33</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="17">
         <v>96</v>
       </c>
-      <c r="J18" s="23"/>
-    </row>
-    <row r="19" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="21" t="s">
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="13">
         <v>2013</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="14">
         <v>24.4</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="14">
         <v>93.6</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="17">
         <v>13</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="17">
         <v>74</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="17">
         <v>29</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="17">
         <v>102</v>
       </c>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="21" t="s">
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="13">
         <v>2013</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="14">
         <v>29.3</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="14">
         <v>93.6</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="17">
         <v>17</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="17">
         <v>85</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="17">
         <v>35</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="17">
         <v>98</v>
       </c>
-      <c r="J20" s="23"/>
-    </row>
-    <row r="21" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="21" t="s">
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="13">
         <v>2014</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="14">
         <v>27.9</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="14">
         <v>93.7</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="17">
         <v>15</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="17">
         <v>72</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="17">
         <v>33</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="17">
         <v>103</v>
       </c>
-      <c r="J21" s="23"/>
-    </row>
-    <row r="22" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="21" t="s">
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="13">
         <v>2014</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="14">
         <v>32.299999999999997</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="14">
         <v>93.6</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="17">
         <v>20</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="17">
         <v>85</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="17">
         <v>38</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="17">
         <v>98</v>
       </c>
-      <c r="J22" s="23"/>
-    </row>
-    <row r="23" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="21" t="s">
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="13">
         <v>2015</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="14">
         <v>28.3</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="14">
         <v>94.8</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="17">
         <v>15</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="17">
         <v>77</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="17">
         <v>34</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="18">
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="21" t="s">
+    <row r="24" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="13">
         <v>2015</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="14">
         <v>32.9</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="14">
         <v>94.9</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="17">
         <v>22</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="17">
         <v>90</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="17">
         <v>38</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="18">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="21" t="s">
+    <row r="25" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="13">
         <v>2016</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="19">
         <v>28.4</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="19">
         <v>93.2</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="17">
         <v>15</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="17">
         <v>78</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="17">
         <v>34</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="17">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="21" t="s">
+    <row r="26" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="13">
         <v>2016</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="14">
         <v>32.700000000000003</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="14">
         <v>93.6</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="17">
         <v>21</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="17">
         <v>88</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="17">
         <v>38</v>
       </c>
-      <c r="I26" s="25">
+      <c r="I26" s="17">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="21" t="s">
+    <row r="27" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="13">
         <v>2017</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="19">
         <v>29.6</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="19">
         <v>93.2</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="17">
         <v>15</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="17">
         <v>71</v>
       </c>
-      <c r="H27" s="25">
+      <c r="H27" s="17">
         <v>37</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="19">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="21" t="s">
+    <row r="28" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="13">
         <v>2017</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="14">
         <v>33.1</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="14">
         <v>93.4</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="17">
         <v>20</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="17">
         <v>84</v>
       </c>
-      <c r="H28" s="25">
+      <c r="H28" s="17">
         <v>40</v>
       </c>
-      <c r="I28" s="26">
+      <c r="I28" s="18">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="21" t="s">
+    <row r="29" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="21">
+      <c r="C29" s="13">
         <v>2018</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="14">
         <v>30.9</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="14">
         <v>92.8</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="19">
         <v>15</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="19">
         <v>73</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="19">
         <v>39</v>
       </c>
-      <c r="I29" s="27">
+      <c r="I29" s="19">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="21" t="s">
+    <row r="30" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="21">
+      <c r="C30" s="13">
         <v>2018</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="14">
         <v>33.6</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="14">
         <v>93</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="17">
         <v>20</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="17">
         <v>82</v>
       </c>
-      <c r="H30" s="25">
-        <v>60</v>
-      </c>
-      <c r="I30" s="26">
+      <c r="H30" s="17">
+        <v>41</v>
+      </c>
+      <c r="I30" s="18">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="13">
+        <v>2019</v>
+      </c>
+      <c r="D31" s="14">
+        <v>32.1</v>
+      </c>
+      <c r="E31" s="14">
+        <v>92.7</v>
+      </c>
+      <c r="F31" s="17">
+        <v>16</v>
+      </c>
+      <c r="G31" s="17">
+        <v>78</v>
+      </c>
+      <c r="H31" s="17">
+        <v>41</v>
+      </c>
+      <c r="I31" s="17">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="21" t="s">
+    <row r="32" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="13">
+        <v>2019</v>
+      </c>
+      <c r="D32" s="14">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E32" s="14">
+        <v>93</v>
+      </c>
+      <c r="F32" s="17">
+        <v>21</v>
+      </c>
+      <c r="G32" s="17">
+        <v>81</v>
+      </c>
+      <c r="H32" s="17">
+        <v>42</v>
+      </c>
+      <c r="I32" s="17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="21">
-        <v>2019</v>
-      </c>
-      <c r="D31" s="22">
-        <v>32.1</v>
-      </c>
-      <c r="E31" s="22">
-        <v>92.7</v>
-      </c>
-      <c r="F31" s="25">
-        <v>16</v>
-      </c>
-      <c r="G31" s="25">
-        <v>78</v>
-      </c>
-      <c r="H31" s="25">
-        <v>41</v>
-      </c>
-      <c r="I31" s="25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="21">
-        <v>2019</v>
-      </c>
-      <c r="D32" s="22">
-        <v>34.299999999999997</v>
-      </c>
-      <c r="E32" s="22">
-        <v>93</v>
-      </c>
-      <c r="F32" s="25">
-        <v>21</v>
-      </c>
-      <c r="G32" s="25">
-        <v>81</v>
-      </c>
-      <c r="H32" s="25">
-        <v>42</v>
-      </c>
-      <c r="I32" s="25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="24">
+      <c r="C33" s="16">
         <f>[1]B1_2020_bearbeitet!B30</f>
         <v>2020</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="14">
         <f>[1]B1_2020_bearbeitet!C30</f>
         <v>32.9</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="14">
         <f>[1]B1_2020_bearbeitet!D30</f>
         <v>92.2</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="17">
         <f>[1]B1_2020_bearbeitet!E30</f>
         <v>17</v>
       </c>
-      <c r="G33" s="25">
+      <c r="G33" s="17">
         <f>[1]B1_2020_bearbeitet!F30</f>
         <v>75</v>
       </c>
-      <c r="H33" s="25">
+      <c r="H33" s="17">
         <f>[1]B1_2020_bearbeitet!G30</f>
         <v>42</v>
       </c>
-      <c r="I33" s="25">
+      <c r="I33" s="17">
         <f>[1]B1_2020_bearbeitet!H30</f>
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="21" t="s">
+    <row r="34" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="16">
         <f>[1]B1_2020_bearbeitet!B31</f>
         <v>2020</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="14">
         <f>[1]B1_2020_bearbeitet!C31</f>
         <v>35</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34" s="14">
         <f>[1]B1_2020_bearbeitet!D31</f>
         <v>92.5</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="17">
         <f>[1]B1_2020_bearbeitet!E31</f>
         <v>21</v>
       </c>
-      <c r="G34" s="25">
+      <c r="G34" s="17">
         <f>[1]B1_2020_bearbeitet!F31</f>
         <v>81</v>
       </c>
-      <c r="H34" s="25">
+      <c r="H34" s="17">
         <f>[1]B1_2020_bearbeitet!G31</f>
         <v>43</v>
       </c>
-      <c r="I34" s="25">
+      <c r="I34" s="17">
         <f>[1]B1_2020_bearbeitet!H31</f>
         <v>99</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B35" s="21"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="30"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="22"/>
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B36" s="31"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="J36" s="7"/>
     </row>
-    <row r="37" spans="2:10" s="24" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="32" t="s">
+    <row r="37" spans="2:10" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B42" s="2" t="s">
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="24" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>